<commit_message>
checking in latest stage of var lists with snowmed
</commit_message>
<xml_diff>
--- a/config/variables_list.xlsx
+++ b/config/variables_list.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mimoor/Desktop/localwork/multicenter-sepsis/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7FFA4DF7-CA46-C84A-AA1A-12F598D9A1BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E019C7-B4D5-D746-9F1F-2A9358132F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="2020" windowWidth="46080" windowHeight="23040"/>
+    <workbookView xWindow="1920" yWindow="900" windowWidth="46080" windowHeight="23040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="variables_list" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="325">
   <si>
     <t>concept</t>
   </si>
@@ -836,12 +836,171 @@
   </si>
   <si>
     <t>sec</t>
+  </si>
+  <si>
+    <t>G/L</t>
+  </si>
+  <si>
+    <t>White blood cell count in blood</t>
+  </si>
+  <si>
+    <t>Fibrinogen level</t>
+  </si>
+  <si>
+    <t>Platelet count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admission age  </t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>Patient sex</t>
+  </si>
+  <si>
+    <t>Blood ionised calcium level</t>
+  </si>
+  <si>
+    <t>Blood sodium level</t>
+  </si>
+  <si>
+    <t>Blood oxygen pressure</t>
+  </si>
+  <si>
+    <t>1013361000000100 | 1000821000000103</t>
+  </si>
+  <si>
+    <t>Plasma albumin level | Serum albumin level</t>
+  </si>
+  <si>
+    <t>1013211000000100 | 1018251000000107</t>
+  </si>
+  <si>
+    <t>Plasma alanine aminotransferase level | Serum alanine aminotransferase level</t>
+  </si>
+  <si>
+    <t>Creatine kinase level</t>
+  </si>
+  <si>
+    <t>Creatine kinase MB isoenzyme level</t>
+  </si>
+  <si>
+    <t>mg/L</t>
+  </si>
+  <si>
+    <t>1106731000000100 | 1106741000000105</t>
+  </si>
+  <si>
+    <t>CRP (C reactive protein) mass concentration in plasma | CRP (C reactive protein) mass concentration in serum</t>
+  </si>
+  <si>
+    <t>1003361000000100 | 1015261000000102</t>
+  </si>
+  <si>
+    <t>Plasma troponin T level | 	Serum troponin T level</t>
+  </si>
+  <si>
+    <t>mL</t>
+  </si>
+  <si>
+    <t>Measure of urine output</t>
+  </si>
+  <si>
+    <t>Basophil percent count in blood</t>
+  </si>
+  <si>
+    <t>Percentage band neutrophil count</t>
+  </si>
+  <si>
+    <t>Eosinophil percent count in blood</t>
+  </si>
+  <si>
+    <t>mm/hr</t>
+  </si>
+  <si>
+    <t>Erythrocyte sedimentation rate</t>
+  </si>
+  <si>
+    <t>Carboxyhaemoglobin level</t>
+  </si>
+  <si>
+    <t>unit ommitted, percent?</t>
+  </si>
+  <si>
+    <t>International normalized ratio</t>
+  </si>
+  <si>
+    <t>Percentage lymphocytes</t>
+  </si>
+  <si>
+    <t>MCH - Mean corpuscular haemoglobin</t>
+  </si>
+  <si>
+    <t>pg</t>
+  </si>
+  <si>
+    <t>MCHC - Mean corpuscular haemoglobin concentration</t>
+  </si>
+  <si>
+    <t>MCV - Mean corpuscular volume</t>
+  </si>
+  <si>
+    <t>fL</t>
+  </si>
+  <si>
+    <t>Methaemoglobin level</t>
+  </si>
+  <si>
+    <t>Neutrophil percent count in blood</t>
+  </si>
+  <si>
+    <t>Prothrombin time</t>
+  </si>
+  <si>
+    <t>Red blood cell count</t>
+  </si>
+  <si>
+    <t>m/uL</t>
+  </si>
+  <si>
+    <t>Red blood cell distribution width</t>
+  </si>
+  <si>
+    <t>Body weight</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>Body height measure</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>SOFA (Sequential Organ Failure Assessment) score</t>
+  </si>
+  <si>
+    <t>qSOFA (quick Sequential Organ Failure Assessment) score</t>
+  </si>
+  <si>
+    <t>Systemic inflammatory response syndrome score</t>
+  </si>
+  <si>
+    <t>National Early Warning Score - Royal College of Physicians</t>
+  </si>
+  <si>
+    <t>Modified early warning score</t>
+  </si>
+  <si>
+    <t>Death</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1688,11 +1847,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N86"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
+      <selection activeCell="L84" sqref="L84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2841,7 +3000,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2860,9 +3019,17 @@
       <c r="F33" t="s">
         <v>67</v>
       </c>
-      <c r="L33" s="3"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K33" t="s">
+        <v>272</v>
+      </c>
+      <c r="L33" s="3">
+        <v>1110441000000100</v>
+      </c>
+      <c r="M33" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2881,9 +3048,17 @@
       <c r="F34" t="s">
         <v>67</v>
       </c>
-      <c r="L34" s="3"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K34" t="s">
+        <v>245</v>
+      </c>
+      <c r="L34" s="3">
+        <v>1019301000000100</v>
+      </c>
+      <c r="M34" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2902,9 +3077,17 @@
       <c r="F35" t="s">
         <v>67</v>
       </c>
-      <c r="L35" s="3"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K35" t="s">
+        <v>272</v>
+      </c>
+      <c r="L35" s="3">
+        <v>1022651000000100</v>
+      </c>
+      <c r="M35" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2923,9 +3106,15 @@
       <c r="F36" t="s">
         <v>82</v>
       </c>
+      <c r="K36" t="s">
+        <v>277</v>
+      </c>
       <c r="L36" s="3"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N36" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2944,9 +3133,14 @@
       <c r="F37" t="s">
         <v>82</v>
       </c>
-      <c r="L37" s="3"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L37" s="3">
+        <v>184100006</v>
+      </c>
+      <c r="M37" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2958,7 +3152,7 @@
       </c>
       <c r="L38" s="3"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2970,7 +3164,7 @@
       </c>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2982,7 +3176,7 @@
       </c>
       <c r="L40" s="3"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2994,7 +3188,7 @@
       </c>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
@@ -3006,7 +3200,7 @@
       </c>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>41</v>
       </c>
@@ -3022,9 +3216,17 @@
       <c r="F43" t="s">
         <v>27</v>
       </c>
-      <c r="L43" s="3"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K43" t="s">
+        <v>261</v>
+      </c>
+      <c r="L43" s="3">
+        <v>1006521000000100</v>
+      </c>
+      <c r="M43" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>42</v>
       </c>
@@ -3040,9 +3242,17 @@
       <c r="F44" t="s">
         <v>27</v>
       </c>
-      <c r="L44" s="3"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K44" t="s">
+        <v>261</v>
+      </c>
+      <c r="L44" s="3">
+        <v>1012681000000100</v>
+      </c>
+      <c r="M44" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>43</v>
       </c>
@@ -3058,9 +3268,17 @@
       <c r="F45" t="s">
         <v>27</v>
       </c>
-      <c r="L45" s="3"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K45" t="s">
+        <v>229</v>
+      </c>
+      <c r="L45" s="3">
+        <v>123820005</v>
+      </c>
+      <c r="M45" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>44</v>
       </c>
@@ -3076,9 +3294,17 @@
       <c r="F46" t="s">
         <v>45</v>
       </c>
-      <c r="L46" s="3"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K46" t="s">
+        <v>268</v>
+      </c>
+      <c r="L46" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="M46" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>45</v>
       </c>
@@ -3094,9 +3320,17 @@
       <c r="F47" t="s">
         <v>45</v>
       </c>
-      <c r="L47" s="3"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K47" t="s">
+        <v>249</v>
+      </c>
+      <c r="L47" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="M47" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>46</v>
       </c>
@@ -3112,9 +3346,17 @@
       <c r="F48" t="s">
         <v>45</v>
       </c>
-      <c r="L48" s="3"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K48" t="s">
+        <v>249</v>
+      </c>
+      <c r="L48" s="3">
+        <v>1028101000000100</v>
+      </c>
+      <c r="M48" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>47</v>
       </c>
@@ -3130,9 +3372,17 @@
       <c r="F49" t="s">
         <v>45</v>
       </c>
-      <c r="L49" s="3"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K49" t="s">
+        <v>266</v>
+      </c>
+      <c r="L49" s="3">
+        <v>1006481000000100</v>
+      </c>
+      <c r="M49" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>48</v>
       </c>
@@ -3148,9 +3398,17 @@
       <c r="F50" t="s">
         <v>45</v>
       </c>
-      <c r="L50" s="3"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K50" t="s">
+        <v>288</v>
+      </c>
+      <c r="L50" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="M50" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>49</v>
       </c>
@@ -3166,9 +3424,17 @@
       <c r="F51" t="s">
         <v>45</v>
       </c>
-      <c r="L51" s="3"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K51" t="s">
+        <v>266</v>
+      </c>
+      <c r="L51" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="M51" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>50</v>
       </c>
@@ -3184,9 +3450,17 @@
       <c r="F52" t="s">
         <v>45</v>
       </c>
-      <c r="L52" s="3"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K52" t="s">
+        <v>293</v>
+      </c>
+      <c r="L52" s="3">
+        <v>364202003</v>
+      </c>
+      <c r="M52" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>51</v>
       </c>
@@ -3202,9 +3476,17 @@
       <c r="F53" t="s">
         <v>67</v>
       </c>
-      <c r="L53" s="3"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K53" t="s">
+        <v>224</v>
+      </c>
+      <c r="L53" s="3">
+        <v>1106101000000100</v>
+      </c>
+      <c r="M53" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>52</v>
       </c>
@@ -3220,9 +3502,17 @@
       <c r="F54" t="s">
         <v>67</v>
       </c>
-      <c r="L54" s="3"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K54" t="s">
+        <v>224</v>
+      </c>
+      <c r="L54" s="3">
+        <v>1083891000000100</v>
+      </c>
+      <c r="M54" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>53</v>
       </c>
@@ -3238,9 +3528,17 @@
       <c r="F55" t="s">
         <v>67</v>
       </c>
-      <c r="L55" s="3"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K55" t="s">
+        <v>224</v>
+      </c>
+      <c r="L55" s="3">
+        <v>1107401000000100</v>
+      </c>
+      <c r="M55" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>54</v>
       </c>
@@ -3256,9 +3554,17 @@
       <c r="F56" t="s">
         <v>67</v>
       </c>
-      <c r="L56" s="3"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K56" t="s">
+        <v>298</v>
+      </c>
+      <c r="L56" s="3">
+        <v>1022511000000100</v>
+      </c>
+      <c r="M56" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>55</v>
       </c>
@@ -3274,9 +3580,17 @@
       <c r="F57" t="s">
         <v>67</v>
       </c>
-      <c r="L57" s="3"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L57" s="3">
+        <v>851001000000100</v>
+      </c>
+      <c r="M57" t="s">
+        <v>300</v>
+      </c>
+      <c r="N57" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>56</v>
       </c>
@@ -3292,9 +3606,14 @@
       <c r="F58" t="s">
         <v>67</v>
       </c>
-      <c r="L58" s="3"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L58">
+        <v>165581004</v>
+      </c>
+      <c r="M58" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>57</v>
       </c>
@@ -3310,9 +3629,17 @@
       <c r="F59" t="s">
         <v>67</v>
       </c>
-      <c r="L59" s="3"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K59" t="s">
+        <v>224</v>
+      </c>
+      <c r="L59" s="3">
+        <v>1015481000000100</v>
+      </c>
+      <c r="M59" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>58</v>
       </c>
@@ -3328,9 +3655,17 @@
       <c r="F60" t="s">
         <v>67</v>
       </c>
-      <c r="L60" s="3"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K60" t="s">
+        <v>305</v>
+      </c>
+      <c r="L60" s="3">
+        <v>1022471000000100</v>
+      </c>
+      <c r="M60" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>59</v>
       </c>
@@ -3346,9 +3681,17 @@
       <c r="F61" t="s">
         <v>67</v>
       </c>
-      <c r="L61" s="3"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K61" t="s">
+        <v>224</v>
+      </c>
+      <c r="L61" s="3">
+        <v>1022481000000100</v>
+      </c>
+      <c r="M61" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>60</v>
       </c>
@@ -3364,9 +3707,17 @@
       <c r="F62" t="s">
         <v>67</v>
       </c>
-      <c r="L62" s="3"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K62" t="s">
+        <v>308</v>
+      </c>
+      <c r="L62" s="3">
+        <v>1022491000000100</v>
+      </c>
+      <c r="M62" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>61</v>
       </c>
@@ -3382,9 +3733,17 @@
       <c r="F63" t="s">
         <v>67</v>
       </c>
-      <c r="L63" s="3"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K63" t="s">
+        <v>224</v>
+      </c>
+      <c r="L63" s="3">
+        <v>1019421000000100</v>
+      </c>
+      <c r="M63" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>62</v>
       </c>
@@ -3400,9 +3759,17 @@
       <c r="F64" t="s">
         <v>67</v>
       </c>
-      <c r="L64" s="3"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K64" t="s">
+        <v>224</v>
+      </c>
+      <c r="L64" s="3">
+        <v>1108061000000100</v>
+      </c>
+      <c r="M64" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>63</v>
       </c>
@@ -3418,9 +3785,17 @@
       <c r="F65" t="s">
         <v>67</v>
       </c>
-      <c r="L65" s="3"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K65" t="s">
+        <v>271</v>
+      </c>
+      <c r="L65" s="3">
+        <v>852471000000107</v>
+      </c>
+      <c r="M65" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>64</v>
       </c>
@@ -3436,9 +3811,17 @@
       <c r="F66" t="s">
         <v>67</v>
       </c>
-      <c r="L66" s="3"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K66" t="s">
+        <v>313</v>
+      </c>
+      <c r="L66" s="3">
+        <v>1022451000000100</v>
+      </c>
+      <c r="M66" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>65</v>
       </c>
@@ -3454,9 +3837,17 @@
       <c r="F67" t="s">
         <v>67</v>
       </c>
-      <c r="L67" s="3"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K67" t="s">
+        <v>224</v>
+      </c>
+      <c r="L67" s="3">
+        <v>993501000000105</v>
+      </c>
+      <c r="M67" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>66</v>
       </c>
@@ -3472,9 +3863,17 @@
       <c r="F68" t="s">
         <v>67</v>
       </c>
-      <c r="L68" s="3"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K68" t="s">
+        <v>229</v>
+      </c>
+      <c r="L68" s="3">
+        <v>250790007</v>
+      </c>
+      <c r="M68" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>67</v>
       </c>
@@ -3490,9 +3889,17 @@
       <c r="F69" t="s">
         <v>82</v>
       </c>
-      <c r="L69" s="3"/>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K69" t="s">
+        <v>316</v>
+      </c>
+      <c r="L69" s="3">
+        <v>27113001</v>
+      </c>
+      <c r="M69" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>68</v>
       </c>
@@ -3508,9 +3915,17 @@
       <c r="F70" t="s">
         <v>82</v>
       </c>
-      <c r="L70" s="3"/>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K70" t="s">
+        <v>318</v>
+      </c>
+      <c r="L70" s="3">
+        <v>50373000</v>
+      </c>
+      <c r="M70" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>69</v>
       </c>
@@ -3528,7 +3943,7 @@
       </c>
       <c r="L71" s="3"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>70</v>
       </c>
@@ -3546,7 +3961,7 @@
       </c>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>71</v>
       </c>
@@ -3564,7 +3979,7 @@
       </c>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>72</v>
       </c>
@@ -3582,7 +3997,7 @@
       </c>
       <c r="L74" s="3"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>73</v>
       </c>
@@ -3600,7 +4015,7 @@
       </c>
       <c r="L75" s="3"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>74</v>
       </c>
@@ -3618,7 +4033,7 @@
       </c>
       <c r="L76" s="3"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>75</v>
       </c>
@@ -3634,9 +4049,14 @@
       <c r="F77" t="s">
         <v>126</v>
       </c>
-      <c r="L77" s="3"/>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L77" s="3">
+        <v>1036771000000100</v>
+      </c>
+      <c r="M77" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>76</v>
       </c>
@@ -3652,9 +4072,14 @@
       <c r="F78" t="s">
         <v>126</v>
       </c>
-      <c r="L78" s="3"/>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L78" s="3">
+        <v>1052131000000100</v>
+      </c>
+      <c r="M78" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>77</v>
       </c>
@@ -3670,9 +4095,14 @@
       <c r="F79" t="s">
         <v>126</v>
       </c>
-      <c r="L79" s="3"/>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L79" s="3">
+        <v>426929000</v>
+      </c>
+      <c r="M79" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>78</v>
       </c>
@@ -3688,9 +4118,14 @@
       <c r="F80" t="s">
         <v>126</v>
       </c>
-      <c r="L80" s="3"/>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L80" s="3">
+        <v>859261000000108</v>
+      </c>
+      <c r="M80" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>79</v>
       </c>
@@ -3706,9 +4141,14 @@
       <c r="F81" t="s">
         <v>126</v>
       </c>
-      <c r="L81" s="3"/>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L81" s="3">
+        <v>445551004</v>
+      </c>
+      <c r="M81" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>80</v>
       </c>
@@ -3724,9 +4164,14 @@
       <c r="F82" t="s">
         <v>143</v>
       </c>
-      <c r="L82" s="3"/>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L82" s="3">
+        <v>419620001</v>
+      </c>
+      <c r="M82" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>81</v>
       </c>
@@ -3744,7 +4189,7 @@
       </c>
       <c r="L83" s="3"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>82</v>
       </c>
@@ -3762,7 +4207,7 @@
       </c>
       <c r="L84" s="3"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>83</v>
       </c>
@@ -3780,8 +4225,14 @@
       </c>
       <c r="L85" s="3"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="L86" s="3"/>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L87" s="3"/>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L88" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>